<commit_message>
First cut for review
</commit_message>
<xml_diff>
--- a/src/test/Species-Summary-Impact-Seychelles.xlsx
+++ b/src/test/Species-Summary-Impact-Seychelles.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SpeciesInformation" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="References" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Species-Impacts'!$D$1:$E$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Species-Impacts'!$E$1:$F$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SpeciesInformation!$B$2:$B$164</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SpeciesLocation!$F$1:$F$283</definedName>
   </definedNames>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3713" uniqueCount="943">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3683" uniqueCount="942">
   <si>
     <t>SpeciesName</t>
   </si>
@@ -2178,9 +2178,6 @@
   </si>
   <si>
     <t>Sus scrofa</t>
-  </si>
-  <si>
-    <t>The entire range of the species is within the Morne Seychellois National Park.</t>
   </si>
   <si>
     <t>Scott's stick insect</t>
@@ -2821,49 +2818,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">The locality where the species is present is dominated by introduced plants, habitat degradation is occurring rapidly, due to invasion by </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Cinnamomum verum</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> and </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Syzygium jambos</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">The main threat is habitat degradation as a result of the invasion by alien plants species, especially </t>
     </r>
     <r>
@@ -2997,9 +2951,6 @@
     <t>Grand Terre</t>
   </si>
   <si>
-    <t>WDPA/GID code</t>
-  </si>
-  <si>
     <t>Mahe</t>
   </si>
   <si>
@@ -3082,6 +3033,12 @@
   </si>
   <si>
     <t>\</t>
+  </si>
+  <si>
+    <t>WDPA code</t>
+  </si>
+  <si>
+    <t>GID code</t>
   </si>
 </sst>
 </file>
@@ -3589,7 +3546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N164"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
@@ -3712,16 +3669,16 @@
         <v>52</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="H3" s="9" t="s">
+        <v>850</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>851</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="J3" s="8" t="s">
         <v>852</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>853</v>
       </c>
       <c r="K3" s="8" t="s">
         <v>79</v>
@@ -3733,7 +3690,7 @@
         <v>32</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3794,19 +3751,19 @@
         <v>50</v>
       </c>
       <c r="F5" s="11" t="s">
+        <v>844</v>
+      </c>
+      <c r="G5" s="12" t="s">
         <v>845</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="H5" s="9" t="s">
         <v>846</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="I5" s="9" t="s">
         <v>847</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>848</v>
-      </c>
       <c r="J5" s="8" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="K5" s="8" t="s">
         <v>79</v>
@@ -3818,7 +3775,7 @@
         <v>32</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3826,7 +3783,7 @@
         <v>33194</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>45</v>
@@ -3841,16 +3798,16 @@
         <v>684</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="H6" s="9" t="s">
+        <v>855</v>
+      </c>
+      <c r="I6" s="9" t="s">
         <v>856</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="J6" s="8" t="s">
         <v>857</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>858</v>
       </c>
       <c r="K6" s="8" t="s">
         <v>79</v>
@@ -3999,19 +3956,19 @@
         <v>51</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="G10" s="12" t="s">
+        <v>836</v>
+      </c>
+      <c r="H10" s="9" t="s">
         <v>837</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="I10" s="9" t="s">
         <v>838</v>
       </c>
-      <c r="I10" s="9" t="s">
-        <v>839</v>
-      </c>
       <c r="J10" s="8" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="K10" s="8" t="s">
         <v>79</v>
@@ -4023,7 +3980,7 @@
         <v>32</v>
       </c>
       <c r="N10" s="8" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -4043,16 +4000,16 @@
         <v>49</v>
       </c>
       <c r="F11" s="18" t="s">
+        <v>756</v>
+      </c>
+      <c r="G11" s="19" t="s">
         <v>757</v>
       </c>
-      <c r="G11" s="19" t="s">
-        <v>758</v>
-      </c>
       <c r="H11" s="9" t="s">
+        <v>747</v>
+      </c>
+      <c r="I11" s="9" t="s">
         <v>748</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>749</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>88</v>
@@ -4064,7 +4021,7 @@
         <v>713</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="N11" s="9" t="s">
         <v>147</v>
@@ -4116,7 +4073,7 @@
         <v>61425</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>44</v>
@@ -4146,13 +4103,13 @@
         <v>59</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="M13" s="8" t="s">
         <v>32</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="14" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -4190,13 +4147,13 @@
         <v>59</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="N14" s="8" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="15" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -4281,7 +4238,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>193404</v>
       </c>
@@ -4325,7 +4282,7 @@
     <row r="18" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="16" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C18" s="18" t="s">
         <v>44</v>
@@ -4337,19 +4294,19 @@
         <v>83</v>
       </c>
       <c r="F18" s="18" t="s">
+        <v>765</v>
+      </c>
+      <c r="G18" s="19" t="s">
         <v>766</v>
       </c>
-      <c r="G18" s="19" t="s">
+      <c r="H18" s="9" t="s">
         <v>767</v>
       </c>
-      <c r="H18" s="9" t="s">
+      <c r="I18" s="9" t="s">
         <v>768</v>
       </c>
-      <c r="I18" s="9" t="s">
-        <v>769</v>
-      </c>
       <c r="J18" s="9" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="K18" s="9" t="s">
         <v>79</v>
@@ -4361,7 +4318,7 @@
         <v>32</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="19" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -4531,7 +4488,7 @@
     <row r="23" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="16" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C23" s="18" t="s">
         <v>44</v>
@@ -4543,19 +4500,19 @@
         <v>83</v>
       </c>
       <c r="F23" s="18" t="s">
+        <v>765</v>
+      </c>
+      <c r="G23" s="19" t="s">
         <v>766</v>
       </c>
-      <c r="G23" s="19" t="s">
-        <v>767</v>
-      </c>
       <c r="H23" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="I23" s="9" t="s">
         <v>798</v>
       </c>
-      <c r="I23" s="9" t="s">
-        <v>799</v>
-      </c>
       <c r="J23" s="9" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="K23" s="9" t="s">
         <v>79</v>
@@ -4567,7 +4524,7 @@
         <v>32</v>
       </c>
       <c r="N23" s="9" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="24" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -4611,7 +4568,7 @@
         <v>32</v>
       </c>
       <c r="N24" s="8" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="25" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -4751,19 +4708,19 @@
         <v>50</v>
       </c>
       <c r="F28" s="11" t="s">
+        <v>862</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>861</v>
+      </c>
+      <c r="H28" s="9" t="s">
         <v>863</v>
       </c>
-      <c r="G28" s="12" t="s">
-        <v>862</v>
-      </c>
-      <c r="H28" s="9" t="s">
+      <c r="I28" s="9" t="s">
         <v>864</v>
       </c>
-      <c r="I28" s="9" t="s">
-        <v>865</v>
-      </c>
       <c r="J28" s="8" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="K28" s="8" t="s">
         <v>79</v>
@@ -4814,7 +4771,7 @@
         <v>32</v>
       </c>
       <c r="N29" s="9" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="30" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -4834,16 +4791,16 @@
         <v>105</v>
       </c>
       <c r="G30" s="12" t="s">
+        <v>866</v>
+      </c>
+      <c r="H30" s="9" t="s">
         <v>867</v>
       </c>
-      <c r="H30" s="9" t="s">
+      <c r="I30" s="9" t="s">
         <v>868</v>
       </c>
-      <c r="I30" s="9" t="s">
-        <v>869</v>
-      </c>
       <c r="J30" s="8" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="K30" s="8" t="s">
         <v>79</v>
@@ -4876,13 +4833,13 @@
         <v>627</v>
       </c>
       <c r="H31" s="9" t="s">
+        <v>770</v>
+      </c>
+      <c r="I31" s="9" t="s">
         <v>771</v>
       </c>
-      <c r="I31" s="9" t="s">
+      <c r="J31" s="9" t="s">
         <v>772</v>
-      </c>
-      <c r="J31" s="9" t="s">
-        <v>773</v>
       </c>
       <c r="K31" s="9" t="s">
         <v>79</v>
@@ -4894,7 +4851,7 @@
         <v>32</v>
       </c>
       <c r="N31" s="9" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="32" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -4976,7 +4933,7 @@
         <v>84</v>
       </c>
       <c r="N33" s="8" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="34" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -5081,13 +5038,13 @@
         <v>52</v>
       </c>
       <c r="G36" s="12" t="s">
+        <v>870</v>
+      </c>
+      <c r="H36" s="9" t="s">
         <v>871</v>
       </c>
-      <c r="H36" s="9" t="s">
+      <c r="I36" s="9" t="s">
         <v>872</v>
-      </c>
-      <c r="I36" s="9" t="s">
-        <v>873</v>
       </c>
       <c r="K36" s="8" t="s">
         <v>79</v>
@@ -5099,7 +5056,7 @@
         <v>32</v>
       </c>
       <c r="N36" s="8" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="37" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -5226,7 +5183,7 @@
         <v>32</v>
       </c>
       <c r="N39" s="9" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="40" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -5934,7 +5891,7 @@
         <v>32</v>
       </c>
       <c r="N56" s="8" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="57" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6013,7 +5970,7 @@
         <v>59</v>
       </c>
       <c r="L58" s="8" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="M58" s="8" t="s">
         <v>32</v>
@@ -6547,13 +6504,13 @@
         <v>59</v>
       </c>
       <c r="L71" s="8" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="M71" s="8" t="s">
         <v>32</v>
       </c>
       <c r="N71" s="8" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="72" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6591,13 +6548,13 @@
         <v>59</v>
       </c>
       <c r="L72" s="8" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="M72" s="8" t="s">
         <v>32</v>
       </c>
       <c r="N72" s="8" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="73" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6635,18 +6592,18 @@
         <v>59</v>
       </c>
       <c r="L73" s="8" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="M73" s="8" t="s">
         <v>32</v>
       </c>
       <c r="N73" s="8" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="74" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="14" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C74" s="11" t="s">
         <v>45</v>
@@ -6658,19 +6615,19 @@
         <v>50</v>
       </c>
       <c r="F74" s="11" t="s">
+        <v>875</v>
+      </c>
+      <c r="G74" s="12" t="s">
         <v>876</v>
       </c>
-      <c r="G74" s="12" t="s">
+      <c r="H74" s="9" t="s">
         <v>877</v>
       </c>
-      <c r="H74" s="9" t="s">
+      <c r="I74" s="9" t="s">
         <v>878</v>
       </c>
-      <c r="I74" s="9" t="s">
-        <v>879</v>
-      </c>
       <c r="J74" s="8" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="K74" s="8" t="s">
         <v>79</v>
@@ -6682,7 +6639,7 @@
         <v>32</v>
       </c>
       <c r="N74" s="8" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="75" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6690,7 +6647,7 @@
         <v>41282</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C75" s="18" t="s">
         <v>44</v>
@@ -6702,19 +6659,19 @@
         <v>83</v>
       </c>
       <c r="F75" s="18" t="s">
+        <v>818</v>
+      </c>
+      <c r="G75" s="19" t="s">
         <v>819</v>
       </c>
-      <c r="G75" s="19" t="s">
-        <v>820</v>
-      </c>
       <c r="H75" s="9" t="s">
+        <v>773</v>
+      </c>
+      <c r="I75" s="9" t="s">
         <v>774</v>
       </c>
-      <c r="I75" s="9" t="s">
+      <c r="J75" s="9" t="s">
         <v>775</v>
-      </c>
-      <c r="J75" s="9" t="s">
-        <v>776</v>
       </c>
       <c r="K75" s="9" t="s">
         <v>79</v>
@@ -6726,7 +6683,7 @@
         <v>32</v>
       </c>
       <c r="N75" s="9" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="76" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6764,13 +6721,13 @@
         <v>59</v>
       </c>
       <c r="L76" s="8" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="M76" s="8" t="s">
         <v>32</v>
       </c>
       <c r="N76" s="8" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="77" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6855,7 +6812,7 @@
         <v>32</v>
       </c>
       <c r="N78" s="8" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="79" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6863,7 +6820,7 @@
         <v>61265</v>
       </c>
       <c r="B79" s="16" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="C79" s="18" t="s">
         <v>44</v>
@@ -6872,31 +6829,31 @@
         <v>46</v>
       </c>
       <c r="E79" s="18" t="s">
+        <v>815</v>
+      </c>
+      <c r="F79" s="18" t="s">
         <v>816</v>
       </c>
-      <c r="F79" s="18" t="s">
+      <c r="G79" s="19" t="s">
         <v>817</v>
       </c>
-      <c r="G79" s="19" t="s">
-        <v>818</v>
-      </c>
       <c r="H79" s="9" t="s">
+        <v>780</v>
+      </c>
+      <c r="I79" s="9" t="s">
         <v>781</v>
       </c>
-      <c r="I79" s="9" t="s">
+      <c r="J79" s="9" t="s">
         <v>782</v>
-      </c>
-      <c r="J79" s="9" t="s">
-        <v>783</v>
       </c>
       <c r="K79" s="9" t="s">
         <v>79</v>
       </c>
       <c r="L79" s="9" t="s">
+        <v>785</v>
+      </c>
+      <c r="M79" s="9" t="s">
         <v>786</v>
-      </c>
-      <c r="M79" s="9" t="s">
-        <v>787</v>
       </c>
       <c r="N79" s="9"/>
     </row>
@@ -7154,7 +7111,7 @@
         <v>13972</v>
       </c>
       <c r="B86" s="16" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C86" s="18" t="s">
         <v>44</v>
@@ -7172,13 +7129,13 @@
         <v>104</v>
       </c>
       <c r="H86" s="9" t="s">
+        <v>812</v>
+      </c>
+      <c r="I86" s="9" t="s">
         <v>813</v>
       </c>
-      <c r="I86" s="9" t="s">
-        <v>814</v>
-      </c>
       <c r="J86" s="9" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="K86" s="9" t="s">
         <v>79</v>
@@ -7190,7 +7147,7 @@
         <v>32</v>
       </c>
       <c r="N86" s="9" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="87" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -7276,7 +7233,7 @@
         <v>32</v>
       </c>
       <c r="N88" s="8" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="89" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -7491,7 +7448,7 @@
         <v>41291</v>
       </c>
       <c r="B94" s="16" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="C94" s="18" t="s">
         <v>44</v>
@@ -7503,16 +7460,16 @@
         <v>83</v>
       </c>
       <c r="F94" s="18" t="s">
+        <v>818</v>
+      </c>
+      <c r="G94" s="19" t="s">
         <v>819</v>
       </c>
-      <c r="G94" s="19" t="s">
-        <v>820</v>
-      </c>
       <c r="H94" s="9" t="s">
+        <v>801</v>
+      </c>
+      <c r="I94" s="9" t="s">
         <v>802</v>
-      </c>
-      <c r="I94" s="9" t="s">
-        <v>803</v>
       </c>
       <c r="J94" s="9" t="s">
         <v>88</v>
@@ -7527,7 +7484,7 @@
         <v>32</v>
       </c>
       <c r="N94" s="9" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="95" spans="1:14" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -7609,7 +7566,7 @@
         <v>149</v>
       </c>
       <c r="L96" s="9" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="M96" s="9" t="s">
         <v>714</v>
@@ -7988,10 +7945,10 @@
         <v>713</v>
       </c>
       <c r="M105" s="8" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="N105" s="8" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="106" spans="1:14" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -8009,16 +7966,16 @@
         <v>50</v>
       </c>
       <c r="F106" s="11" t="s">
+        <v>844</v>
+      </c>
+      <c r="G106" s="12" t="s">
         <v>845</v>
       </c>
-      <c r="G106" s="12" t="s">
-        <v>846</v>
-      </c>
       <c r="H106" s="9" t="s">
+        <v>880</v>
+      </c>
+      <c r="I106" s="9" t="s">
         <v>881</v>
-      </c>
-      <c r="I106" s="9" t="s">
-        <v>882</v>
       </c>
       <c r="J106" s="8"/>
       <c r="K106" s="8" t="s">
@@ -8205,7 +8162,7 @@
         <v>17902</v>
       </c>
       <c r="B111" s="14" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C111" s="11" t="s">
         <v>44</v>
@@ -8217,19 +8174,19 @@
         <v>51</v>
       </c>
       <c r="F111" s="11" t="s">
+        <v>900</v>
+      </c>
+      <c r="G111" s="12" t="s">
         <v>901</v>
       </c>
-      <c r="G111" s="12" t="s">
-        <v>902</v>
-      </c>
       <c r="H111" s="9" t="s">
+        <v>753</v>
+      </c>
+      <c r="I111" s="9" t="s">
         <v>754</v>
       </c>
-      <c r="I111" s="9" t="s">
+      <c r="J111" s="8" t="s">
         <v>755</v>
-      </c>
-      <c r="J111" s="8" t="s">
-        <v>756</v>
       </c>
       <c r="K111" s="8" t="s">
         <v>58</v>
@@ -8241,7 +8198,7 @@
         <v>32</v>
       </c>
       <c r="N111" s="8" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="112" spans="1:14" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -8405,11 +8362,11 @@
         <v>693</v>
       </c>
       <c r="L115" s="8" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="M115" s="8"/>
       <c r="N115" s="8" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="116" spans="1:14" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -8724,13 +8681,13 @@
         <v>106</v>
       </c>
       <c r="H123" s="9" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="I123" s="9" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="J123" s="8" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="K123" s="8" t="s">
         <v>79</v>
@@ -8797,19 +8754,19 @@
         <v>50</v>
       </c>
       <c r="F125" s="11" t="s">
+        <v>844</v>
+      </c>
+      <c r="G125" s="12" t="s">
         <v>845</v>
       </c>
-      <c r="G125" s="12" t="s">
-        <v>846</v>
-      </c>
       <c r="H125" s="9" t="s">
+        <v>886</v>
+      </c>
+      <c r="I125" s="9" t="s">
         <v>887</v>
       </c>
-      <c r="I125" s="9" t="s">
-        <v>888</v>
-      </c>
       <c r="J125" s="8" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="K125" s="8" t="s">
         <v>79</v>
@@ -8929,10 +8886,10 @@
         <v>98</v>
       </c>
       <c r="I128" s="9" t="s">
+        <v>803</v>
+      </c>
+      <c r="J128" s="9" t="s">
         <v>804</v>
-      </c>
-      <c r="J128" s="9" t="s">
-        <v>805</v>
       </c>
       <c r="K128" s="9" t="s">
         <v>79</v>
@@ -8944,7 +8901,7 @@
         <v>32</v>
       </c>
       <c r="N128" s="9" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="129" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -9032,7 +8989,7 @@
         <v>32</v>
       </c>
       <c r="N130" s="8" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="131" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -9118,12 +9075,12 @@
         <v>32</v>
       </c>
       <c r="N132" s="8" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="133" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B133" s="14" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="C133" s="11" t="s">
         <v>45</v>
@@ -9138,16 +9095,16 @@
         <v>624</v>
       </c>
       <c r="G133" s="12" t="s">
+        <v>892</v>
+      </c>
+      <c r="H133" s="9" t="s">
         <v>893</v>
       </c>
-      <c r="H133" s="9" t="s">
+      <c r="I133" s="9" t="s">
         <v>894</v>
       </c>
-      <c r="I133" s="9" t="s">
+      <c r="J133" s="8" t="s">
         <v>895</v>
-      </c>
-      <c r="J133" s="8" t="s">
-        <v>896</v>
       </c>
       <c r="K133" s="8" t="s">
         <v>79</v>
@@ -9296,10 +9253,10 @@
         <v>645</v>
       </c>
       <c r="F137" s="11" t="s">
+        <v>834</v>
+      </c>
+      <c r="G137" s="12" t="s">
         <v>835</v>
-      </c>
-      <c r="G137" s="12" t="s">
-        <v>836</v>
       </c>
       <c r="H137" s="9" t="s">
         <v>402</v>
@@ -9584,19 +9541,19 @@
         <v>49</v>
       </c>
       <c r="F144" s="18" t="s">
+        <v>756</v>
+      </c>
+      <c r="G144" s="19" t="s">
         <v>757</v>
       </c>
-      <c r="G144" s="19" t="s">
-        <v>758</v>
-      </c>
       <c r="H144" s="9" t="s">
+        <v>750</v>
+      </c>
+      <c r="I144" s="9" t="s">
         <v>751</v>
       </c>
-      <c r="I144" s="9" t="s">
+      <c r="J144" s="9" t="s">
         <v>752</v>
-      </c>
-      <c r="J144" s="9" t="s">
-        <v>753</v>
       </c>
       <c r="K144" s="9" t="s">
         <v>152</v>
@@ -9605,7 +9562,7 @@
         <v>713</v>
       </c>
       <c r="M144" s="9" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="N144" s="9" t="s">
         <v>715</v>
@@ -9710,19 +9667,19 @@
         <v>83</v>
       </c>
       <c r="F147" s="18" t="s">
+        <v>810</v>
+      </c>
+      <c r="G147" s="19" t="s">
         <v>811</v>
       </c>
-      <c r="G147" s="19" t="s">
-        <v>812</v>
-      </c>
       <c r="H147" s="9" t="s">
+        <v>789</v>
+      </c>
+      <c r="I147" s="9" t="s">
         <v>790</v>
       </c>
-      <c r="I147" s="9" t="s">
-        <v>791</v>
-      </c>
       <c r="J147" s="9" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="K147" s="9" t="s">
         <v>79</v>
@@ -9734,7 +9691,7 @@
         <v>32</v>
       </c>
       <c r="N147" s="9" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="148" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -9796,25 +9753,25 @@
         <v>83</v>
       </c>
       <c r="F149" s="11" t="s">
+        <v>902</v>
+      </c>
+      <c r="G149" s="12" t="s">
         <v>903</v>
       </c>
-      <c r="G149" s="12" t="s">
-        <v>904</v>
-      </c>
       <c r="H149" s="9" t="s">
+        <v>897</v>
+      </c>
+      <c r="I149" s="9" t="s">
         <v>898</v>
       </c>
-      <c r="I149" s="9" t="s">
+      <c r="J149" s="8" t="s">
         <v>899</v>
-      </c>
-      <c r="J149" s="8" t="s">
-        <v>900</v>
       </c>
       <c r="K149" s="8" t="s">
         <v>79</v>
       </c>
       <c r="N149" s="8" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="150" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -10165,22 +10122,22 @@
         <v>668</v>
       </c>
       <c r="G158" s="12" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="H158" s="9" t="s">
+        <v>905</v>
+      </c>
+      <c r="I158" s="9" t="s">
         <v>906</v>
       </c>
-      <c r="I158" s="9" t="s">
+      <c r="J158" s="8" t="s">
         <v>907</v>
-      </c>
-      <c r="J158" s="8" t="s">
-        <v>908</v>
       </c>
       <c r="K158" s="8" t="s">
         <v>79</v>
       </c>
       <c r="N158" s="8" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="159" spans="1:14" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -10347,7 +10304,7 @@
         <v>32</v>
       </c>
       <c r="N162" s="8" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="163" spans="1:14" s="10" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -10382,7 +10339,7 @@
   <dimension ref="A1:K284"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A47" sqref="A47:XFD48"/>
     </sheetView>
   </sheetViews>
@@ -10445,7 +10402,7 @@
         <v>161</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G2" s="7">
         <v>10450</v>
@@ -10471,7 +10428,7 @@
         <v>161</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G3" s="7">
         <v>10450</v>
@@ -10497,10 +10454,10 @@
         <v>161</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>942</v>
+        <v>939</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>128</v>
@@ -10514,7 +10471,7 @@
         <v>138</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>23</v>
@@ -10523,7 +10480,7 @@
         <v>161</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="G5" s="7">
         <v>231720</v>
@@ -10549,7 +10506,7 @@
         <v>138</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>23</v>
@@ -10558,7 +10515,7 @@
         <v>161</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="G6" s="7">
         <v>231720</v>
@@ -10584,7 +10541,7 @@
         <v>138</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>23</v>
@@ -10593,7 +10550,7 @@
         <v>161</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="G7" s="7">
         <v>231720</v>
@@ -10619,7 +10576,7 @@
         <v>138</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>23</v>
@@ -10654,7 +10611,7 @@
         <v>138</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>23</v>
@@ -10689,7 +10646,7 @@
         <v>138</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>23</v>
@@ -10724,7 +10681,7 @@
         <v>138</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>23</v>
@@ -10750,7 +10707,7 @@
         <v>138</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>23</v>
@@ -10785,7 +10742,7 @@
         <v>138</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>23</v>
@@ -10820,7 +10777,7 @@
         <v>138</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>23</v>
@@ -10855,13 +10812,13 @@
         <v>138</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>23</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="G15" s="9">
         <v>187330</v>
@@ -10884,7 +10841,7 @@
         <v>161</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G16" s="7">
         <v>10450</v>
@@ -10907,7 +10864,7 @@
         <v>161</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G17" s="7">
         <v>37110</v>
@@ -10947,7 +10904,7 @@
         <v>161</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G19" s="7">
         <v>10450</v>
@@ -10970,7 +10927,7 @@
         <v>161</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G20" s="7">
         <v>37110</v>
@@ -11010,7 +10967,7 @@
         <v>161</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="G22" s="7">
         <v>24420</v>
@@ -11033,7 +10990,7 @@
         <v>161</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G23" s="7">
         <v>37110</v>
@@ -11056,7 +11013,7 @@
         <v>161</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G24" s="7">
         <v>37110</v>
@@ -11143,7 +11100,7 @@
         <v>161</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="G27" s="7">
         <v>231720</v>
@@ -11175,7 +11132,7 @@
         <v>161</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="G28" s="7">
         <v>231720</v>
@@ -11207,7 +11164,7 @@
         <v>161</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="G29" s="7">
         <v>231720</v>
@@ -11236,7 +11193,7 @@
         <v>23</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="G30" s="7">
         <v>224450</v>
@@ -11268,13 +11225,13 @@
         <v>160</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="G31" s="7">
         <v>261980</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="J31" s="9" t="s">
         <v>146</v>
@@ -11300,7 +11257,7 @@
         <v>161</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G32" s="7">
         <v>10450</v>
@@ -11341,7 +11298,7 @@
         <v>61425</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>16</v>
@@ -11353,7 +11310,7 @@
         <v>161</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G34" s="7">
         <v>10450</v>
@@ -11364,7 +11321,7 @@
         <v>61425</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>16</v>
@@ -11376,7 +11333,7 @@
         <v>161</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="G35" s="7">
         <v>24420</v>
@@ -11387,7 +11344,7 @@
         <v>61425</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>16</v>
@@ -11399,7 +11356,7 @@
         <v>161</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="G36" s="7">
         <v>24420</v>
@@ -11413,7 +11370,7 @@
         <v>61425</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>16</v>
@@ -11425,7 +11382,7 @@
         <v>161</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G37" s="7">
         <v>37110</v>
@@ -11436,7 +11393,7 @@
         <v>61425</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>16</v>
@@ -11457,13 +11414,13 @@
         <v>135</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D39" s="9" t="s">
         <v>23</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="G39" s="7">
         <v>12730</v>
@@ -11489,13 +11446,13 @@
         <v>135</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D40" s="9" t="s">
         <v>23</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="G40" s="7">
         <v>12730</v>
@@ -11521,13 +11478,13 @@
         <v>135</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>23</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="G41" s="7">
         <v>12730</v>
@@ -11553,13 +11510,13 @@
         <v>135</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D42" s="9" t="s">
         <v>23</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="G42" s="7">
         <v>12730</v>
@@ -11594,7 +11551,7 @@
         <v>161</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G43" s="7">
         <v>37110</v>
@@ -11617,7 +11574,7 @@
         <v>161</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G44" s="7">
         <v>37110</v>
@@ -11643,7 +11600,7 @@
         <v>161</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G45" s="7">
         <v>37110</v>
@@ -11684,7 +11641,7 @@
         <v>161</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G47" s="7">
         <v>10450</v>
@@ -11707,7 +11664,7 @@
         <v>161</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G48" s="7">
         <v>10450</v>
@@ -11733,7 +11690,7 @@
         <v>161</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G49" s="7">
         <v>37110</v>
@@ -11756,7 +11713,7 @@
         <v>161</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G50" s="7">
         <v>37110</v>
@@ -11782,7 +11739,7 @@
         <v>161</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="G51" s="7">
         <v>53540</v>
@@ -11805,7 +11762,7 @@
         <v>161</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="G52" s="7">
         <v>24420</v>
@@ -11828,7 +11785,7 @@
         <v>161</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="G53" s="7">
         <v>24420</v>
@@ -11854,7 +11811,7 @@
         <v>161</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G54" s="7">
         <v>37110</v>
@@ -11877,7 +11834,7 @@
         <v>161</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G55" s="7">
         <v>37110</v>
@@ -11903,7 +11860,7 @@
         <v>161</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G56" s="7">
         <v>10450</v>
@@ -11944,7 +11901,7 @@
         <v>161</v>
       </c>
       <c r="F58" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G58" s="7">
         <v>10450</v>
@@ -11967,7 +11924,7 @@
         <v>161</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="G59" s="7">
         <v>24420</v>
@@ -11990,7 +11947,7 @@
         <v>161</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="G60" s="7">
         <v>24420</v>
@@ -12016,7 +11973,7 @@
         <v>161</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G61" s="7">
         <v>37110</v>
@@ -12039,7 +11996,7 @@
         <v>161</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="G62" s="7">
         <v>132230</v>
@@ -12080,7 +12037,7 @@
         <v>161</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G64" s="7">
         <v>10450</v>
@@ -12103,7 +12060,7 @@
         <v>161</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G65" s="7">
         <v>37110</v>
@@ -12144,7 +12101,7 @@
         <v>161</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G67" s="7">
         <v>37110</v>
@@ -12167,7 +12124,7 @@
         <v>161</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G68" s="7">
         <v>37110</v>
@@ -12193,7 +12150,7 @@
         <v>161</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G69" s="7">
         <v>10450</v>
@@ -12216,7 +12173,7 @@
         <v>161</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G70" s="7">
         <v>37110</v>
@@ -12257,7 +12214,7 @@
         <v>161</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G72" s="7">
         <v>37110</v>
@@ -12280,7 +12237,7 @@
         <v>161</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G73" s="7">
         <v>37110</v>
@@ -12306,7 +12263,7 @@
         <v>161</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G74" s="7">
         <v>37110</v>
@@ -12329,7 +12286,7 @@
         <v>161</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G75" s="7">
         <v>37110</v>
@@ -12355,7 +12312,7 @@
         <v>161</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G76" s="7">
         <v>10450</v>
@@ -12378,7 +12335,7 @@
         <v>161</v>
       </c>
       <c r="F77" s="9" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="G77" s="7">
         <v>24420</v>
@@ -12401,7 +12358,7 @@
         <v>161</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G78" s="7">
         <v>37110</v>
@@ -12442,7 +12399,7 @@
         <v>161</v>
       </c>
       <c r="F80" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G80" s="7">
         <v>10450</v>
@@ -12465,7 +12422,7 @@
         <v>161</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G81" s="7">
         <v>37110</v>
@@ -12488,7 +12445,7 @@
         <v>161</v>
       </c>
       <c r="F82" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G82" s="7">
         <v>10450</v>
@@ -12520,7 +12477,7 @@
         <v>141</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D84" s="9" t="s">
         <v>23</v>
@@ -12529,7 +12486,7 @@
         <v>161</v>
       </c>
       <c r="F84" s="7" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="G84" s="7">
         <v>231720</v>
@@ -12546,7 +12503,7 @@
         <v>141</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D85" s="9" t="s">
         <v>23</v>
@@ -12569,7 +12526,7 @@
         <v>141</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D86" s="9" t="s">
         <v>23</v>
@@ -12604,7 +12561,7 @@
         <v>141</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D87" s="9" t="s">
         <v>23</v>
@@ -12639,7 +12596,7 @@
         <v>141</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D88" s="9" t="s">
         <v>23</v>
@@ -12674,7 +12631,7 @@
         <v>141</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D89" s="9" t="s">
         <v>23</v>
@@ -12697,7 +12654,7 @@
         <v>141</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D90" s="9" t="s">
         <v>23</v>
@@ -12732,7 +12689,7 @@
         <v>141</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D91" s="9" t="s">
         <v>23</v>
@@ -12767,7 +12724,7 @@
         <v>141</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D92" s="9" t="s">
         <v>23</v>
@@ -12802,13 +12759,13 @@
         <v>141</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D93" s="9" t="s">
         <v>23</v>
       </c>
       <c r="F93" s="9" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="G93" s="9">
         <v>187330</v>
@@ -12822,7 +12779,7 @@
         <v>141</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D94" s="9" t="s">
         <v>23</v>
@@ -12831,7 +12788,7 @@
         <v>161</v>
       </c>
       <c r="F94" s="7" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="G94" s="7">
         <v>132660</v>
@@ -12845,7 +12802,7 @@
         <v>141</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D95" s="9" t="s">
         <v>23</v>
@@ -12854,7 +12811,7 @@
         <v>161</v>
       </c>
       <c r="F95" s="7" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="G95" s="7">
         <v>132660</v>
@@ -12880,7 +12837,7 @@
         <v>141</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D96" s="9" t="s">
         <v>23</v>
@@ -12889,7 +12846,7 @@
         <v>161</v>
       </c>
       <c r="F96" s="7" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="G96" s="7">
         <v>132660</v>
@@ -12924,7 +12881,7 @@
         <v>161</v>
       </c>
       <c r="F97" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G97" s="7">
         <v>10450</v>
@@ -12947,7 +12904,7 @@
         <v>161</v>
       </c>
       <c r="F98" s="9" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="G98" s="7">
         <v>24420</v>
@@ -12970,7 +12927,7 @@
         <v>161</v>
       </c>
       <c r="F99" s="9" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="G99" s="7">
         <v>24420</v>
@@ -12996,7 +12953,7 @@
         <v>161</v>
       </c>
       <c r="F100" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G100" s="7">
         <v>37110</v>
@@ -13055,7 +13012,7 @@
         <v>161</v>
       </c>
       <c r="F103" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G103" s="7">
         <v>10450</v>
@@ -13078,7 +13035,7 @@
         <v>161</v>
       </c>
       <c r="F104" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G104" s="7">
         <v>37110</v>
@@ -13110,13 +13067,13 @@
         <v>136</v>
       </c>
       <c r="C106" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D106" s="9" t="s">
         <v>23</v>
       </c>
       <c r="F106" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="G106" s="7">
         <v>12730</v>
@@ -13130,13 +13087,13 @@
         <v>136</v>
       </c>
       <c r="C107" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D107" s="9" t="s">
         <v>23</v>
       </c>
       <c r="F107" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="G107" s="7">
         <v>12730</v>
@@ -13162,13 +13119,13 @@
         <v>136</v>
       </c>
       <c r="C108" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D108" s="9" t="s">
         <v>23</v>
       </c>
       <c r="F108" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="G108" s="7">
         <v>12730</v>
@@ -13194,13 +13151,13 @@
         <v>136</v>
       </c>
       <c r="C109" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D109" s="9" t="s">
         <v>23</v>
       </c>
       <c r="F109" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="G109" s="7">
         <v>12730</v>
@@ -13226,13 +13183,13 @@
         <v>136</v>
       </c>
       <c r="C110" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D110" s="9" t="s">
         <v>23</v>
       </c>
       <c r="F110" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="G110" s="7">
         <v>12730</v>
@@ -13258,7 +13215,7 @@
         <v>136</v>
       </c>
       <c r="C111" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D111" s="9" t="s">
         <v>23</v>
@@ -13278,7 +13235,7 @@
         <v>136</v>
       </c>
       <c r="C112" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D112" s="9" t="s">
         <v>23</v>
@@ -13298,7 +13255,7 @@
         <v>136</v>
       </c>
       <c r="C113" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D113" s="9" t="s">
         <v>23</v>
@@ -13318,7 +13275,7 @@
         <v>136</v>
       </c>
       <c r="C114" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D114" s="9" t="s">
         <v>23</v>
@@ -13338,7 +13295,7 @@
         <v>136</v>
       </c>
       <c r="C115" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D115" s="9" t="s">
         <v>23</v>
@@ -13358,7 +13315,7 @@
         <v>136</v>
       </c>
       <c r="C116" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D116" s="9" t="s">
         <v>23</v>
@@ -13375,7 +13332,7 @@
         <v>136</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D117" s="9" t="s">
         <v>23</v>
@@ -13392,7 +13349,7 @@
         <v>136</v>
       </c>
       <c r="C118" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D118" s="9" t="s">
         <v>23</v>
@@ -13409,13 +13366,13 @@
         <v>136</v>
       </c>
       <c r="C119" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D119" s="9" t="s">
         <v>23</v>
       </c>
       <c r="F119" s="9" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
     </row>
     <row r="120" spans="1:7" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -13435,7 +13392,7 @@
         <v>161</v>
       </c>
       <c r="F120" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G120" s="7">
         <v>10450</v>
@@ -13458,7 +13415,7 @@
         <v>161</v>
       </c>
       <c r="F121" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G121" s="7">
         <v>37110</v>
@@ -13492,7 +13449,7 @@
         <v>459</v>
       </c>
       <c r="C123" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D123" s="9" t="s">
         <v>23</v>
@@ -13501,7 +13458,7 @@
         <v>161</v>
       </c>
       <c r="F123" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G123" s="7">
         <v>37110</v>
@@ -13524,7 +13481,7 @@
         <v>161</v>
       </c>
       <c r="F124" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G124" s="7">
         <v>10450</v>
@@ -13547,7 +13504,7 @@
         <v>161</v>
       </c>
       <c r="F125" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G125" s="7">
         <v>37110</v>
@@ -13570,7 +13527,7 @@
         <v>161</v>
       </c>
       <c r="F126" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G126" s="7">
         <v>10450</v>
@@ -13593,7 +13550,7 @@
         <v>161</v>
       </c>
       <c r="F127" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G127" s="7">
         <v>37110</v>
@@ -13633,7 +13590,7 @@
         <v>161</v>
       </c>
       <c r="F129" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G129" s="7">
         <v>10450</v>
@@ -13656,7 +13613,7 @@
         <v>161</v>
       </c>
       <c r="F130" s="9" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="G130" s="7">
         <v>24420</v>
@@ -13670,7 +13627,7 @@
         <v>139</v>
       </c>
       <c r="C131" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D131" s="9" t="s">
         <v>23</v>
@@ -13679,7 +13636,7 @@
         <v>161</v>
       </c>
       <c r="F131" s="9" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="G131" s="7">
         <v>282640</v>
@@ -13705,7 +13662,7 @@
         <v>139</v>
       </c>
       <c r="C132" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D132" s="9" t="s">
         <v>23</v>
@@ -13714,7 +13671,7 @@
         <v>161</v>
       </c>
       <c r="F132" s="9" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="G132" s="7">
         <v>282640</v>
@@ -13740,7 +13697,7 @@
         <v>139</v>
       </c>
       <c r="C133" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D133" s="9" t="s">
         <v>23</v>
@@ -13749,7 +13706,7 @@
         <v>161</v>
       </c>
       <c r="F133" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G133" s="7">
         <v>10450</v>
@@ -13775,7 +13732,7 @@
         <v>139</v>
       </c>
       <c r="C134" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D134" s="9" t="s">
         <v>23</v>
@@ -13784,7 +13741,7 @@
         <v>161</v>
       </c>
       <c r="F134" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G134" s="7">
         <v>10450</v>
@@ -13810,7 +13767,7 @@
         <v>139</v>
       </c>
       <c r="C135" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D135" s="9" t="s">
         <v>23</v>
@@ -13819,7 +13776,7 @@
         <v>161</v>
       </c>
       <c r="F135" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G135" s="7">
         <v>10450</v>
@@ -13845,7 +13802,7 @@
         <v>139</v>
       </c>
       <c r="C136" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D136" s="9" t="s">
         <v>23</v>
@@ -13854,7 +13811,7 @@
         <v>161</v>
       </c>
       <c r="F136" s="9" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="G136" s="7">
         <v>24420</v>
@@ -13880,7 +13837,7 @@
         <v>139</v>
       </c>
       <c r="C137" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D137" s="9" t="s">
         <v>23</v>
@@ -13889,7 +13846,7 @@
         <v>161</v>
       </c>
       <c r="F137" s="9" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="G137" s="7">
         <v>24420</v>
@@ -13915,7 +13872,7 @@
         <v>139</v>
       </c>
       <c r="C138" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D138" s="9" t="s">
         <v>23</v>
@@ -13944,7 +13901,7 @@
         <v>139</v>
       </c>
       <c r="C139" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D139" s="9" t="s">
         <v>23</v>
@@ -13973,7 +13930,7 @@
         <v>139</v>
       </c>
       <c r="C140" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D140" s="9" t="s">
         <v>23</v>
@@ -14002,7 +13959,7 @@
         <v>139</v>
       </c>
       <c r="C141" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D141" s="9" t="s">
         <v>23</v>
@@ -14031,7 +13988,7 @@
         <v>139</v>
       </c>
       <c r="C142" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D142" s="9" t="s">
         <v>23</v>
@@ -14058,7 +14015,7 @@
         <v>139</v>
       </c>
       <c r="C143" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D143" s="9" t="s">
         <v>23</v>
@@ -14072,7 +14029,7 @@
         <v>142</v>
       </c>
       <c r="C144" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D144" s="9" t="s">
         <v>23</v>
@@ -14107,7 +14064,7 @@
         <v>142</v>
       </c>
       <c r="C145" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D145" s="9" t="s">
         <v>23</v>
@@ -14142,7 +14099,7 @@
         <v>142</v>
       </c>
       <c r="C146" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D146" s="9" t="s">
         <v>23</v>
@@ -14177,7 +14134,7 @@
         <v>142</v>
       </c>
       <c r="C147" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D147" s="9" t="s">
         <v>23</v>
@@ -14212,7 +14169,7 @@
         <v>142</v>
       </c>
       <c r="C148" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D148" s="9" t="s">
         <v>23</v>
@@ -14247,7 +14204,7 @@
         <v>142</v>
       </c>
       <c r="C149" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D149" s="9" t="s">
         <v>23</v>
@@ -14282,7 +14239,7 @@
         <v>142</v>
       </c>
       <c r="C150" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D150" s="9" t="s">
         <v>23</v>
@@ -14317,7 +14274,7 @@
         <v>142</v>
       </c>
       <c r="C151" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D151" s="9" t="s">
         <v>23</v>
@@ -14349,7 +14306,7 @@
         <v>142</v>
       </c>
       <c r="C152" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D152" s="9" t="s">
         <v>23</v>
@@ -14381,7 +14338,7 @@
         <v>142</v>
       </c>
       <c r="C153" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D153" s="9" t="s">
         <v>23</v>
@@ -14410,7 +14367,7 @@
         <v>142</v>
       </c>
       <c r="C154" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D154" s="9" t="s">
         <v>23</v>
@@ -14448,7 +14405,7 @@
         <v>161</v>
       </c>
       <c r="F155" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G155" s="7">
         <v>10450</v>
@@ -14471,7 +14428,7 @@
         <v>161</v>
       </c>
       <c r="F156" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G156" s="7">
         <v>37110</v>
@@ -14494,7 +14451,7 @@
         <v>161</v>
       </c>
       <c r="F157" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G157" s="7">
         <v>10450</v>
@@ -14517,7 +14474,7 @@
         <v>161</v>
       </c>
       <c r="F158" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G158" s="7">
         <v>37110</v>
@@ -14540,7 +14497,7 @@
         <v>161</v>
       </c>
       <c r="F159" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G159" s="7">
         <v>37110</v>
@@ -14566,7 +14523,7 @@
         <v>161</v>
       </c>
       <c r="F160" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G160" s="7">
         <v>10450</v>
@@ -14589,7 +14546,7 @@
         <v>161</v>
       </c>
       <c r="F161" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G161" s="7">
         <v>10450</v>
@@ -14612,7 +14569,7 @@
         <v>161</v>
       </c>
       <c r="F162" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G162" s="7">
         <v>37110</v>
@@ -14635,7 +14592,7 @@
         <v>161</v>
       </c>
       <c r="F163" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G163" s="7">
         <v>37110</v>
@@ -14658,7 +14615,7 @@
         <v>161</v>
       </c>
       <c r="F164" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G164" s="7">
         <v>10450</v>
@@ -14681,7 +14638,7 @@
         <v>161</v>
       </c>
       <c r="F165" s="9" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="G165" s="7">
         <v>24420</v>
@@ -14704,7 +14661,7 @@
         <v>161</v>
       </c>
       <c r="F166" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G166" s="7">
         <v>37110</v>
@@ -14727,7 +14684,7 @@
         <v>161</v>
       </c>
       <c r="F167" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G167" s="7">
         <v>10450</v>
@@ -14750,7 +14707,7 @@
         <v>161</v>
       </c>
       <c r="F168" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G168" s="7">
         <v>37110</v>
@@ -14764,7 +14721,7 @@
         <v>472</v>
       </c>
       <c r="C169" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D169" s="9" t="s">
         <v>23</v>
@@ -14773,7 +14730,7 @@
         <v>161</v>
       </c>
       <c r="F169" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G169" s="7">
         <v>10450</v>
@@ -14787,7 +14744,7 @@
         <v>472</v>
       </c>
       <c r="C170" s="9" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D170" s="9" t="s">
         <v>23</v>
@@ -14796,7 +14753,7 @@
         <v>161</v>
       </c>
       <c r="F170" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G170" s="7">
         <v>37110</v>
@@ -14819,7 +14776,7 @@
         <v>161</v>
       </c>
       <c r="F171" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G171" s="7">
         <v>10450</v>
@@ -14842,7 +14799,7 @@
         <v>161</v>
       </c>
       <c r="F172" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G172" s="7">
         <v>37110</v>
@@ -14865,7 +14822,7 @@
         <v>161</v>
       </c>
       <c r="F173" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G173" s="7">
         <v>37110</v>
@@ -14888,7 +14845,7 @@
         <v>161</v>
       </c>
       <c r="F174" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G174" s="7">
         <v>10450</v>
@@ -14911,7 +14868,7 @@
         <v>161</v>
       </c>
       <c r="F175" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G175" s="7">
         <v>37110</v>
@@ -14934,7 +14891,7 @@
         <v>161</v>
       </c>
       <c r="F176" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G176" s="7">
         <v>10450</v>
@@ -14957,7 +14914,7 @@
         <v>161</v>
       </c>
       <c r="F177" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G177" s="7">
         <v>37110</v>
@@ -14980,7 +14937,7 @@
         <v>161</v>
       </c>
       <c r="F178" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G178" s="7">
         <v>10450</v>
@@ -15003,7 +14960,7 @@
         <v>161</v>
       </c>
       <c r="F179" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G179" s="7">
         <v>10450</v>
@@ -15026,7 +14983,7 @@
         <v>161</v>
       </c>
       <c r="F180" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G180" s="7">
         <v>37110</v>
@@ -15049,7 +15006,7 @@
         <v>161</v>
       </c>
       <c r="F181" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G181" s="7">
         <v>10450</v>
@@ -15095,7 +15052,7 @@
         <v>161</v>
       </c>
       <c r="F183" s="7" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="G183" s="7">
         <v>53540</v>
@@ -15118,7 +15075,7 @@
         <v>161</v>
       </c>
       <c r="F184" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G184" s="7">
         <v>10450</v>
@@ -15141,7 +15098,7 @@
         <v>161</v>
       </c>
       <c r="F185" s="9" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="G185" s="7">
         <v>24420</v>
@@ -15164,7 +15121,7 @@
         <v>161</v>
       </c>
       <c r="F186" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G186" s="7">
         <v>37110</v>
@@ -15187,7 +15144,7 @@
         <v>161</v>
       </c>
       <c r="F187" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G187" s="7">
         <v>10450</v>
@@ -15210,7 +15167,7 @@
         <v>161</v>
       </c>
       <c r="F188" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G188" s="7">
         <v>10450</v>
@@ -15384,7 +15341,7 @@
         <v>23</v>
       </c>
       <c r="F203" s="9" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="G203" s="9">
         <v>12730</v>
@@ -15413,7 +15370,7 @@
         <v>23</v>
       </c>
       <c r="F204" s="9" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="G204" s="9">
         <v>12730</v>
@@ -15442,7 +15399,7 @@
         <v>23</v>
       </c>
       <c r="F205" s="9" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="G205" s="9">
         <v>12730</v>
@@ -15471,7 +15428,7 @@
         <v>23</v>
       </c>
       <c r="F206" s="9" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="G206" s="9">
         <v>12730</v>
@@ -15572,7 +15529,7 @@
         <v>161</v>
       </c>
       <c r="F213" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G213" s="7">
         <v>10450</v>
@@ -15607,7 +15564,7 @@
         <v>161</v>
       </c>
       <c r="F214" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G214" s="7">
         <v>10450</v>
@@ -15642,7 +15599,7 @@
         <v>161</v>
       </c>
       <c r="F215" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G215" s="7">
         <v>10450</v>
@@ -15819,7 +15776,7 @@
         <v>17902</v>
       </c>
       <c r="B230" s="16" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="D230" s="9" t="s">
         <v>23</v>
@@ -16183,7 +16140,7 @@
         <v>161</v>
       </c>
       <c r="F259" s="7" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="G259" s="7">
         <v>231720</v>
@@ -16215,7 +16172,7 @@
         <v>161</v>
       </c>
       <c r="F260" s="7" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="G260" s="7">
         <v>231720</v>
@@ -16247,7 +16204,7 @@
         <v>161</v>
       </c>
       <c r="F261" s="7" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="G261" s="7">
         <v>231720</v>
@@ -16276,7 +16233,7 @@
         <v>23</v>
       </c>
       <c r="F262" s="7" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="G262" s="7">
         <v>224450</v>
@@ -16337,7 +16294,7 @@
         <v>160</v>
       </c>
       <c r="F264" s="9" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="G264" s="9">
         <v>264900</v>
@@ -16502,7 +16459,7 @@
         <v>161</v>
       </c>
       <c r="F276" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G276" s="9">
         <v>10450</v>
@@ -16556,7 +16513,7 @@
         <v>161</v>
       </c>
       <c r="F279" s="9" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="G279" s="7">
         <v>282640</v>
@@ -16588,7 +16545,7 @@
         <v>161</v>
       </c>
       <c r="F280" s="9" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="G280" s="7">
         <v>282640</v>
@@ -16620,7 +16577,7 @@
         <v>161</v>
       </c>
       <c r="F281" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G281" s="7">
         <v>10450</v>
@@ -16652,7 +16609,7 @@
         <v>161</v>
       </c>
       <c r="F282" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G282" s="7">
         <v>10450</v>
@@ -16684,7 +16641,7 @@
         <v>161</v>
       </c>
       <c r="F283" s="9" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G283" s="7">
         <v>10450</v>
@@ -16717,11 +16674,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -16771,10 +16728,10 @@
         <v>10450</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>938</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="8" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="8" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="28">
         <v>106007629</v>
       </c>
@@ -16788,7 +16745,7 @@
         <v>231720</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="8" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -16805,7 +16762,7 @@
         <v>10450</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="8" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -16822,7 +16779,7 @@
         <v>10450</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="8" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -16833,13 +16790,13 @@
         <v>440</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D6" s="27">
         <v>24420</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>941</v>
+        <v>938</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="8" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -16849,295 +16806,131 @@
       <c r="B7" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="C7" s="27" t="s">
-        <v>114</v>
+      <c r="C7" s="25" t="s">
+        <v>920</v>
       </c>
       <c r="D7" s="27">
-        <v>874280</v>
+        <v>261980</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="8" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="28">
-        <v>106003294</v>
-      </c>
-      <c r="B8" s="29" t="s">
-        <v>133</v>
-      </c>
-      <c r="C8" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="D8" s="27">
-        <v>231720</v>
+        <v>199526</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="28">
+        <v>6937</v>
       </c>
       <c r="E8" s="28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>61425</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>734</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="7">
+        <v>10450</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" s="8" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28">
-        <v>106003294</v>
-      </c>
-      <c r="B9" s="29" t="s">
-        <v>133</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="D9" s="27">
-        <v>224450</v>
-      </c>
-      <c r="E9" s="28" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="8" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="28">
-        <v>106003294</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>133</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>922</v>
-      </c>
-      <c r="D10" s="27">
-        <v>261980</v>
-      </c>
-      <c r="E10" s="28" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="8" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="28">
-        <v>199526</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="28" t="s">
+      <c r="F9" s="8" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>106003735</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>758</v>
+      </c>
+      <c r="D10" s="7">
+        <v>12730</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>740</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>199630</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>441</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>911</v>
+      </c>
+      <c r="D11" s="7">
+        <v>37110</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>918</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>199489</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>442</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="28">
+      <c r="D12" s="7">
         <v>10450</v>
       </c>
-      <c r="E11" s="28" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="8" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="28">
-        <v>199526</v>
-      </c>
-      <c r="B12" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="28">
-        <v>6937</v>
-      </c>
-      <c r="E12" s="28" t="s">
-        <v>85</v>
+      <c r="E12" s="8" t="s">
+        <v>919</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>745</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
-        <v>199526</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" s="7">
-        <v>10450</v>
+        <v>33549</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="8">
+        <v>6937</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>917</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
-        <v>61425</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>735</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" s="7">
-        <v>10450</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>918</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
-        <v>61425</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>735</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>913</v>
-      </c>
-      <c r="D15" s="7">
-        <v>24420</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>918</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
-        <v>61425</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>735</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>912</v>
-      </c>
-      <c r="D16" s="7">
-        <v>37110</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>918</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
-        <v>106003735</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>759</v>
-      </c>
-      <c r="D17" s="7">
-        <v>12730</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>741</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>919</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
-        <v>199630</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>441</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>912</v>
-      </c>
-      <c r="D18" s="7">
-        <v>37110</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>920</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
-        <v>199489</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>442</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>912</v>
-      </c>
-      <c r="D19" s="7">
-        <v>37110</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>921</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
-        <v>199489</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>442</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D20" s="7">
-        <v>10450</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>921</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
-        <v>33549</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21" s="8">
-        <v>10450</v>
-      </c>
-      <c r="E21" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
-        <v>33549</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="8">
-        <v>6937</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
+    <row r="14" spans="1:7" s="8" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sortState ref="A2:G19">
     <sortCondition ref="B2:B19"/>
@@ -17148,28 +16941,28 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="A13:G13"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="15.85546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="19" style="4" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" style="13" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" style="4" customWidth="1"/>
-    <col min="8" max="10" width="9.140625" style="4"/>
-    <col min="11" max="11" width="21.85546875" style="4" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" style="4" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="4"/>
+    <col min="3" max="4" width="19" style="4" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="4" customWidth="1"/>
+    <col min="9" max="11" width="9.140625" style="4"/>
+    <col min="12" max="12" width="21.85546875" style="4" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" style="4" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>75</v>
       </c>
@@ -17177,22 +16970,25 @@
         <v>73</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>935</v>
+        <v>940</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>941</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="10" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25">
         <v>168135</v>
       </c>
@@ -17202,313 +16998,341 @@
       <c r="C2" s="25">
         <v>6937</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="25"/>
+      <c r="E2" s="26" t="s">
         <v>437</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="F2" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="G2" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="H2" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="16"/>
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>
-    </row>
-    <row r="3" spans="1:14" s="10" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O2" s="9"/>
+    </row>
+    <row r="3" spans="1:15" s="10" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="25">
-        <v>168135</v>
+        <v>199524</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>936</v>
-      </c>
-      <c r="C3" s="27">
-        <v>10450</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>437</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C3" s="25">
+        <v>6937</v>
+      </c>
+      <c r="D3" s="25"/>
       <c r="E3" s="26" t="s">
+        <v>438</v>
+      </c>
+      <c r="F3" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="G3" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="H3" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="9"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="16"/>
       <c r="M3" s="9"/>
       <c r="N3" s="9"/>
-    </row>
-    <row r="4" spans="1:14" s="10" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O3" s="9"/>
+    </row>
+    <row r="4" spans="1:15" s="10" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25">
-        <v>199526</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>924</v>
-      </c>
-      <c r="C4" s="27">
-        <v>231720</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>138</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>716</v>
-      </c>
-      <c r="F4" s="25" t="s">
-        <v>19</v>
+        <v>199519</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="25">
+        <v>6937</v>
+      </c>
+      <c r="D4" s="25"/>
+      <c r="E4" s="26" t="s">
+        <v>439</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>25</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="9"/>
-      <c r="K4" s="16"/>
+        <v>165</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="9"/>
+      <c r="L4" s="16"/>
       <c r="M4" s="9"/>
       <c r="N4" s="9"/>
-    </row>
-    <row r="5" spans="1:14" s="10" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O4" s="9"/>
+    </row>
+    <row r="5" spans="1:15" s="10" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25">
-        <v>199526</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>939</v>
-      </c>
-      <c r="C5" s="27">
-        <v>419990</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>138</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>716</v>
-      </c>
-      <c r="F5" s="25" t="s">
-        <v>19</v>
+        <v>168135</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>933</v>
+      </c>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27">
+        <v>19631</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>437</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>25</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="9"/>
-      <c r="K5" s="16"/>
+        <v>165</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="9"/>
+      <c r="L5" s="16"/>
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
-    </row>
-    <row r="6" spans="1:14" s="10" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O5" s="9"/>
+    </row>
+    <row r="6" spans="1:15" s="10" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25">
         <v>199524</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="25">
-        <v>6937</v>
-      </c>
-      <c r="D6" s="26" t="s">
+        <v>933</v>
+      </c>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27">
+        <v>19631</v>
+      </c>
+      <c r="E6" s="26" t="s">
         <v>438</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="F6" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="G6" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="H6" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="9"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="16"/>
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
-    </row>
-    <row r="7" spans="1:14" s="10" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O6" s="9"/>
+    </row>
+    <row r="7" spans="1:15" s="10" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25">
-        <v>199524</v>
+        <v>199519</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>936</v>
-      </c>
-      <c r="C7" s="27">
-        <v>10450</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>438</v>
+        <v>933</v>
+      </c>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27">
+        <v>19631</v>
       </c>
       <c r="E7" s="26" t="s">
+        <v>439</v>
+      </c>
+      <c r="F7" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="G7" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="G7" s="25" t="s">
+      <c r="H7" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="9"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="16"/>
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
-    </row>
-    <row r="8" spans="1:14" s="10" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O7" s="9"/>
+    </row>
+    <row r="8" spans="1:15" s="10" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25">
-        <v>199519</v>
+        <v>199551</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="25">
-        <v>6937</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>439</v>
-      </c>
+        <v>930</v>
+      </c>
+      <c r="C8" s="27">
+        <v>6938</v>
+      </c>
+      <c r="D8" s="27"/>
       <c r="E8" s="26" t="s">
+        <v>440</v>
+      </c>
+      <c r="F8" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="G8" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="H8" s="25" t="s">
         <v>15</v>
       </c>
+      <c r="I8" s="9"/>
       <c r="J8" s="9"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="16"/>
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
-    </row>
-    <row r="9" spans="1:14" s="10" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O8" s="9"/>
+    </row>
+    <row r="9" spans="1:15" s="10" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25">
-        <v>199519</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>936</v>
+        <v>199551</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>931</v>
       </c>
       <c r="C9" s="27">
-        <v>10450</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>439</v>
-      </c>
+        <v>62230</v>
+      </c>
+      <c r="D9" s="27"/>
       <c r="E9" s="26" t="s">
+        <v>440</v>
+      </c>
+      <c r="F9" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="G9" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="H9" s="25" t="s">
         <v>15</v>
       </c>
+      <c r="I9" s="9"/>
       <c r="J9" s="9"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="16"/>
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
-    </row>
-    <row r="10" spans="1:14" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O9" s="9"/>
+    </row>
+    <row r="10" spans="1:15" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="25">
-        <v>199551</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>932</v>
+        <v>199526</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>922</v>
       </c>
       <c r="C10" s="27">
-        <v>24420</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>440</v>
-      </c>
+        <v>6941</v>
+      </c>
+      <c r="D10" s="27"/>
       <c r="E10" s="26" t="s">
-        <v>25</v>
+        <v>138</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>165</v>
+        <v>716</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="K10" s="16"/>
-    </row>
-    <row r="11" spans="1:14" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="H10" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="10"/>
+    </row>
+    <row r="11" spans="1:15" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25">
-        <v>199551</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>555</v>
-      </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="26" t="s">
-        <v>440</v>
-      </c>
+        <v>199526</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>936</v>
+      </c>
+      <c r="C11" s="27">
+        <v>6939</v>
+      </c>
+      <c r="D11" s="27"/>
       <c r="E11" s="26" t="s">
-        <v>25</v>
+        <v>138</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>165</v>
+        <v>716</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="K11" s="16"/>
-    </row>
-    <row r="12" spans="1:14" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="10"/>
+    </row>
+    <row r="12" spans="1:15" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="25">
         <v>199551</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>557</v>
-      </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="26" t="s">
+        <v>555</v>
+      </c>
+      <c r="C12" s="25">
+        <v>62230</v>
+      </c>
+      <c r="D12" s="25"/>
+      <c r="E12" s="26" t="s">
         <v>440</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="F12" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="G12" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="G12" s="25" t="s">
+      <c r="H12" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="K12" s="16"/>
-    </row>
-    <row r="13" spans="1:14" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L12" s="16"/>
+    </row>
+    <row r="13" spans="1:15" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="25">
         <v>199551</v>
       </c>
-      <c r="B13" s="27" t="s">
-        <v>933</v>
-      </c>
-      <c r="C13" s="27">
-        <v>37110</v>
-      </c>
-      <c r="D13" s="26" t="s">
+      <c r="B13" s="25" t="s">
+        <v>557</v>
+      </c>
+      <c r="C13" s="25">
+        <v>6938</v>
+      </c>
+      <c r="D13" s="25"/>
+      <c r="E13" s="26" t="s">
         <v>440</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="F13" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="25" t="s">
+      <c r="G13" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="G13" s="25" t="s">
+      <c r="H13" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
     </row>
   </sheetData>
-  <sortState ref="A2:G176">
-    <sortCondition ref="D2:D176"/>
+  <sortState ref="A1:O13">
+    <sortCondition ref="C2:C13"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17550,7 +17374,7 @@
         <v>221</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -17558,7 +17382,7 @@
         <v>194</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -17566,10 +17390,10 @@
         <v>33194</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -17577,7 +17401,7 @@
         <v>356</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -17585,7 +17409,7 @@
         <v>356</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -17596,7 +17420,7 @@
         <v>133</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -17607,7 +17431,7 @@
         <v>22</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -17615,10 +17439,10 @@
         <v>61425</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -17629,7 +17453,7 @@
         <v>135</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -17640,7 +17464,7 @@
         <v>441</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -17651,31 +17475,31 @@
         <v>442</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="16" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="16" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="16" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -17683,7 +17507,7 @@
         <v>401</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -17691,7 +17515,7 @@
         <v>25</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -17699,7 +17523,7 @@
         <v>381</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -17707,7 +17531,7 @@
         <v>184</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -17718,7 +17542,7 @@
         <v>141</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -17729,7 +17553,7 @@
         <v>141</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -17740,7 +17564,7 @@
         <v>136</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -18075,10 +17899,10 @@
     </row>
     <row r="53" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="16" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="54" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -18086,10 +17910,10 @@
         <v>41282</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="55" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -18097,10 +17921,10 @@
         <v>41282</v>
       </c>
       <c r="B55" s="21" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="56" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -18108,10 +17932,10 @@
         <v>61265</v>
       </c>
       <c r="B56" s="16" t="s">
+        <v>783</v>
+      </c>
+      <c r="C56" s="9" t="s">
         <v>784</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>785</v>
       </c>
     </row>
     <row r="57" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -18119,10 +17943,10 @@
         <v>13972</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="58" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -18141,10 +17965,10 @@
         <v>41291</v>
       </c>
       <c r="B59" s="22" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="60" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -18163,7 +17987,7 @@
         <v>309</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="62" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -18171,10 +17995,10 @@
         <v>17902</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
     </row>
     <row r="63" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -18182,10 +18006,10 @@
         <v>17902</v>
       </c>
       <c r="B63" s="16" t="s">
+        <v>824</v>
+      </c>
+      <c r="C63" s="9" t="s">
         <v>825</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="64" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -18193,7 +18017,7 @@
         <v>195</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="65" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -18201,7 +18025,7 @@
         <v>213</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="66" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -18212,7 +18036,7 @@
         <v>222</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="67" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -18223,15 +18047,15 @@
         <v>28</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="68" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="23" t="s">
+        <v>890</v>
+      </c>
+      <c r="C68" s="9" t="s">
         <v>891</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>892</v>
       </c>
     </row>
     <row r="69" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -18242,7 +18066,7 @@
         <v>134</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
     </row>
     <row r="70" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -18253,7 +18077,7 @@
         <v>134</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="71" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -18264,7 +18088,7 @@
         <v>716</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="72" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -18272,7 +18096,7 @@
         <v>17</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="73" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -18283,7 +18107,7 @@
         <v>298</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="74" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -18294,7 +18118,7 @@
         <v>214</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="75" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -18305,7 +18129,7 @@
         <v>26</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="76" spans="1:3" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>